<commit_message>
effect objects system added and image boundary optimized
</commit_message>
<xml_diff>
--- a/out/production/JavaFXFinalProject/MagicalBattle/loader/Ability.xlsx
+++ b/out/production/JavaFXFinalProject/MagicalBattle/loader/Ability.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pudding\JavaFXFinalProject\src\MagicalBattle\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pudding\JavaFXFinalProject\src\MagicalBattle\loader\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -538,7 +538,7 @@
                   <c:v>0.42857142857142866</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.33333333333333331</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -605,7 +605,7 @@
                   <c:v>0.36363636363636365</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.375</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.8666666666666667</c:v>
@@ -614,7 +614,7 @@
                   <c:v>0.21428571428571433</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.16666666666666666</c:v>
+                  <c:v>0.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -681,7 +681,7 @@
                   <c:v>0.81818181818181823</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.875</c:v>
+                  <c:v>0.95</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.2</c:v>
@@ -690,7 +690,7 @@
                   <c:v>0.28571428571428581</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.16666666666666666</c:v>
+                  <c:v>0.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -757,7 +757,7 @@
                   <c:v>0.54545454545454541</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.75</c:v>
+                  <c:v>0.82499999999999996</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.26666666666666666</c:v>
@@ -766,7 +766,7 @@
                   <c:v>0.42857142857142866</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.33333333333333331</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -853,7 +853,7 @@
                   <c:v>0.36363636363636365</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.5</c:v>
+                  <c:v>0.52500000000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.13333333333333333</c:v>
@@ -862,7 +862,7 @@
                   <c:v>0.64285714285714279</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.66666666666666663</c:v>
+                  <c:v>0.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -929,7 +929,7 @@
                   <c:v>0.54545454545454541</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.65</c:v>
+                  <c:v>0.7</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.4</c:v>
@@ -938,7 +938,7 @@
                   <c:v>0.28571428571428581</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.16666666666666666</c:v>
+                  <c:v>0.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -954,11 +954,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="-24"/>
-        <c:axId val="1538819744"/>
-        <c:axId val="1538821376"/>
+        <c:axId val="-1966577264"/>
+        <c:axId val="-1772082528"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1538819744"/>
+        <c:axId val="-1966577264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1001,7 +1001,7 @@
             <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1538821376"/>
+        <c:crossAx val="-1772082528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1009,7 +1009,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1538821376"/>
+        <c:axId val="-1772082528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1060,7 +1060,7 @@
             <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1538819744"/>
+        <c:crossAx val="-1966577264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1984,7 +1984,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.4"/>
@@ -2068,7 +2068,7 @@
       </c>
       <c r="H3" s="6">
         <f t="shared" si="0"/>
-        <v>0.33333333333333331</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.4">
@@ -2085,7 +2085,7 @@
         <v>120</v>
       </c>
       <c r="E4" s="7">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F4" s="7">
         <v>13</v>
@@ -2112,7 +2112,7 @@
       </c>
       <c r="E5" s="7">
         <f t="shared" si="1"/>
-        <v>0.375</v>
+        <v>0.4</v>
       </c>
       <c r="F5" s="7">
         <f t="shared" si="1"/>
@@ -2124,7 +2124,7 @@
       </c>
       <c r="H5" s="7">
         <f t="shared" si="1"/>
-        <v>0.16666666666666666</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.4">
@@ -2141,7 +2141,7 @@
         <v>220</v>
       </c>
       <c r="E6" s="8">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="F6" s="8">
         <v>3</v>
@@ -2168,7 +2168,7 @@
       </c>
       <c r="E7" s="8">
         <f t="shared" si="2"/>
-        <v>0.875</v>
+        <v>0.95</v>
       </c>
       <c r="F7" s="8">
         <f t="shared" si="2"/>
@@ -2180,7 +2180,7 @@
       </c>
       <c r="H7" s="8">
         <f t="shared" si="2"/>
-        <v>0.16666666666666666</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.4">
@@ -2197,7 +2197,7 @@
         <v>160</v>
       </c>
       <c r="E8" s="14">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="F8" s="14">
         <v>4</v>
@@ -2224,7 +2224,7 @@
       </c>
       <c r="E9" s="14">
         <f t="shared" si="3"/>
-        <v>0.75</v>
+        <v>0.82499999999999996</v>
       </c>
       <c r="F9" s="14">
         <f t="shared" si="3"/>
@@ -2236,7 +2236,7 @@
       </c>
       <c r="H9" s="14">
         <f t="shared" si="3"/>
-        <v>0.33333333333333331</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.4">
@@ -2253,7 +2253,7 @@
         <v>120</v>
       </c>
       <c r="E10" s="9">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F10" s="9">
         <v>2</v>
@@ -2262,7 +2262,7 @@
         <v>1.1499999999999999</v>
       </c>
       <c r="H10" s="9">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.4">
@@ -2280,7 +2280,7 @@
       </c>
       <c r="E11" s="9">
         <f t="shared" si="4"/>
-        <v>0.5</v>
+        <v>0.52500000000000002</v>
       </c>
       <c r="F11" s="9">
         <f t="shared" si="4"/>
@@ -2292,7 +2292,7 @@
       </c>
       <c r="H11" s="9">
         <f t="shared" si="4"/>
-        <v>0.66666666666666663</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.4">
@@ -2309,7 +2309,7 @@
         <v>160</v>
       </c>
       <c r="E12" s="12">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F12" s="12">
         <v>6</v>
@@ -2336,7 +2336,7 @@
       </c>
       <c r="E13" s="12">
         <f t="shared" si="5"/>
-        <v>0.65</v>
+        <v>0.7</v>
       </c>
       <c r="F13" s="12">
         <f t="shared" si="5"/>
@@ -2348,7 +2348,7 @@
       </c>
       <c r="H13" s="12">
         <f t="shared" si="5"/>
-        <v>0.16666666666666666</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.4">
@@ -2372,7 +2372,7 @@
         <v>1.4</v>
       </c>
       <c r="H14" s="10">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.4">
@@ -2426,7 +2426,7 @@
       </c>
       <c r="H16" s="10">
         <f t="shared" si="6"/>
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>